<commit_message>
Added self assessment and comments from Alex
</commit_message>
<xml_diff>
--- a/files/assesments/firstround/assesments-jacob.xlsx
+++ b/files/assesments/firstround/assesments-jacob.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lanes\OneDrive\Dokumenter\uni\2. semester\epic\files\assesments\firstround\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobvejlinjensen/Honeyjar/files/assesments/firstround/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22240" windowHeight="13440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Peer  and self assessment" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="37">
   <si>
     <t>Self assesment</t>
   </si>
@@ -130,12 +130,29 @@
   </si>
   <si>
     <t>Robert</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research, Hardware setup </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I have been active in the weekly online Discord meetings - both in 
+terms of planning (Adding discussion points to the meeting agenda, taking responsibility for leading a group discussion or a walkthrough of conducted work, etc) 
+I have been reading through literature and materials uploaded
+to GiT by other project group members, and actively been adding comments and suggestions. I have been uploading relevant materials to
+GiT as well.  
+I have been responding fairly quickly to messages, both private and group announcements, on the discord platform. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Active collaborator, Motivated </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -583,15 +600,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C124"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.125" customWidth="1"/>
-    <col min="2" max="2" width="21.625" customWidth="1"/>
-    <col min="3" max="3" width="64.75" customWidth="1"/>
+    <col min="1" max="1" width="40.1640625" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="64.6640625" customWidth="1"/>
     <col min="7" max="7" width="54" customWidth="1"/>
   </cols>
   <sheetData>
@@ -606,12 +623,16 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7"/>
+      <c r="B2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="3" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -624,7 +645,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>31</v>
       </c>
@@ -633,10 +654,14 @@
     </row>
     <row r="5" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="4"/>
+        <v>33</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -645,42 +670,42 @@
       <c r="B6" s="6"/>
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="4"/>
     </row>
-    <row r="13" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
@@ -691,78 +716,78 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="4"/>
     </row>
-    <row r="18" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="4"/>
     </row>
-    <row r="22" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B23" s="6"/>
       <c r="C23" s="4"/>
     </row>
-    <row r="24" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>18</v>
       </c>
@@ -773,78 +798,78 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="4"/>
     </row>
-    <row r="27" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B27" s="6"/>
       <c r="C27" s="4"/>
     </row>
-    <row r="28" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B28" s="6"/>
       <c r="C28" s="4"/>
     </row>
-    <row r="29" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B29" s="6"/>
       <c r="C29" s="4"/>
     </row>
-    <row r="30" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B30" s="6"/>
       <c r="C30" s="4"/>
     </row>
-    <row r="31" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B31" s="6"/>
       <c r="C31" s="4"/>
     </row>
-    <row r="32" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B32" s="6"/>
       <c r="C32" s="4"/>
     </row>
-    <row r="33" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B33" s="6"/>
       <c r="C33" s="4"/>
     </row>
-    <row r="34" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B34" s="6"/>
       <c r="C34" s="4"/>
     </row>
-    <row r="35" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B35" s="6"/>
       <c r="C35" s="4"/>
     </row>
-    <row r="36" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>19</v>
       </c>
@@ -855,78 +880,78 @@
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B38" s="6"/>
       <c r="C38" s="4"/>
     </row>
-    <row r="39" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B39" s="6"/>
       <c r="C39" s="4"/>
     </row>
-    <row r="40" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B40" s="6"/>
       <c r="C40" s="4"/>
     </row>
-    <row r="41" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B41" s="6"/>
       <c r="C41" s="4"/>
     </row>
-    <row r="42" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B42" s="6"/>
       <c r="C42" s="4"/>
     </row>
-    <row r="43" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B43" s="6"/>
       <c r="C43" s="4"/>
     </row>
-    <row r="44" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B44" s="6"/>
       <c r="C44" s="4"/>
     </row>
-    <row r="45" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B45" s="6"/>
       <c r="C45" s="4"/>
     </row>
-    <row r="46" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B46" s="6"/>
       <c r="C46" s="4"/>
     </row>
-    <row r="47" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B47" s="6"/>
       <c r="C47" s="4"/>
     </row>
-    <row r="48" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="49" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
         <v>20</v>
       </c>
@@ -937,78 +962,78 @@
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B50" s="6"/>
       <c r="C50" s="4"/>
     </row>
-    <row r="51" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B51" s="6"/>
       <c r="C51" s="4"/>
     </row>
-    <row r="52" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B52" s="6"/>
       <c r="C52" s="4"/>
     </row>
-    <row r="53" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B53" s="6"/>
       <c r="C53" s="4"/>
     </row>
-    <row r="54" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B54" s="6"/>
       <c r="C54" s="4"/>
     </row>
-    <row r="55" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B55" s="6"/>
       <c r="C55" s="4"/>
     </row>
-    <row r="56" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B56" s="6"/>
       <c r="C56" s="4"/>
     </row>
-    <row r="57" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B57" s="6"/>
       <c r="C57" s="4"/>
     </row>
-    <row r="58" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B58" s="6"/>
       <c r="C58" s="4"/>
     </row>
-    <row r="59" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B59" s="6"/>
       <c r="C59" s="4"/>
     </row>
-    <row r="60" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
         <v>21</v>
       </c>
@@ -1019,78 +1044,84 @@
         <v>14</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B62" s="6"/>
+      <c r="B62" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="C62" s="4"/>
     </row>
-    <row r="63" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B63" s="6"/>
-      <c r="C63" s="4"/>
-    </row>
-    <row r="64" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B64" s="6"/>
       <c r="C64" s="4"/>
     </row>
-    <row r="65" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B65" s="6"/>
       <c r="C65" s="4"/>
     </row>
-    <row r="66" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B66" s="6"/>
       <c r="C66" s="4"/>
     </row>
-    <row r="67" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B67" s="6"/>
       <c r="C67" s="4"/>
     </row>
-    <row r="68" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B68" s="6"/>
       <c r="C68" s="4"/>
     </row>
-    <row r="69" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B69" s="6"/>
       <c r="C69" s="4"/>
     </row>
-    <row r="70" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B70" s="6"/>
       <c r="C70" s="4"/>
     </row>
-    <row r="71" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B71" s="6"/>
       <c r="C71" s="4"/>
     </row>
-    <row r="72" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="73" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="5" t="s">
         <v>22</v>
       </c>
@@ -1101,78 +1132,78 @@
         <v>14</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B74" s="6"/>
       <c r="C74" s="4"/>
     </row>
-    <row r="75" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B75" s="6"/>
       <c r="C75" s="4"/>
     </row>
-    <row r="76" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B76" s="6"/>
       <c r="C76" s="4"/>
     </row>
-    <row r="77" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B77" s="6"/>
       <c r="C77" s="4"/>
     </row>
-    <row r="78" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B78" s="6"/>
       <c r="C78" s="4"/>
     </row>
-    <row r="79" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B79" s="6"/>
       <c r="C79" s="4"/>
     </row>
-    <row r="80" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B80" s="6"/>
       <c r="C80" s="4"/>
     </row>
-    <row r="81" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B81" s="6"/>
       <c r="C81" s="4"/>
     </row>
-    <row r="82" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B82" s="6"/>
       <c r="C82" s="4"/>
     </row>
-    <row r="83" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B83" s="6"/>
       <c r="C83" s="4"/>
     </row>
-    <row r="84" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="85" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="85" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="5" t="s">
         <v>23</v>
       </c>
@@ -1183,78 +1214,78 @@
         <v>14</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B86" s="6"/>
       <c r="C86" s="4"/>
     </row>
-    <row r="87" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B87" s="6"/>
       <c r="C87" s="4"/>
     </row>
-    <row r="88" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B88" s="6"/>
       <c r="C88" s="4"/>
     </row>
-    <row r="89" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B89" s="6"/>
       <c r="C89" s="4"/>
     </row>
-    <row r="90" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B90" s="6"/>
       <c r="C90" s="4"/>
     </row>
-    <row r="91" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B91" s="6"/>
       <c r="C91" s="4"/>
     </row>
-    <row r="92" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B92" s="6"/>
       <c r="C92" s="4"/>
     </row>
-    <row r="93" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B93" s="6"/>
       <c r="C93" s="4"/>
     </row>
-    <row r="94" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B94" s="6"/>
       <c r="C94" s="4"/>
     </row>
-    <row r="95" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B95" s="6"/>
       <c r="C95" s="4"/>
     </row>
-    <row r="96" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="97" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="97" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="5" t="s">
         <v>24</v>
       </c>
@@ -1265,78 +1296,78 @@
         <v>14</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B98" s="6"/>
       <c r="C98" s="4"/>
     </row>
-    <row r="99" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B99" s="6"/>
       <c r="C99" s="4"/>
     </row>
-    <row r="100" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B100" s="6"/>
       <c r="C100" s="4"/>
     </row>
-    <row r="101" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B101" s="6"/>
       <c r="C101" s="4"/>
     </row>
-    <row r="102" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B102" s="6"/>
       <c r="C102" s="4"/>
     </row>
-    <row r="103" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B103" s="6"/>
       <c r="C103" s="4"/>
     </row>
-    <row r="104" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B104" s="6"/>
       <c r="C104" s="4"/>
     </row>
-    <row r="105" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B105" s="6"/>
       <c r="C105" s="4"/>
     </row>
-    <row r="106" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B106" s="6"/>
       <c r="C106" s="4"/>
     </row>
-    <row r="107" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B107" s="6"/>
       <c r="C107" s="4"/>
     </row>
-    <row r="108" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="109" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="109" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="5" t="s">
         <v>25</v>
       </c>
@@ -1347,99 +1378,99 @@
         <v>14</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B110" s="6"/>
       <c r="C110" s="4"/>
     </row>
-    <row r="111" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B111" s="6"/>
       <c r="C111" s="4"/>
     </row>
-    <row r="112" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B112" s="6"/>
       <c r="C112" s="4"/>
     </row>
-    <row r="113" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B113" s="6"/>
       <c r="C113" s="4"/>
     </row>
-    <row r="114" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B114" s="6"/>
       <c r="C114" s="4"/>
     </row>
-    <row r="115" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B115" s="6"/>
       <c r="C115" s="4"/>
     </row>
-    <row r="116" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B116" s="6"/>
       <c r="C116" s="4"/>
     </row>
-    <row r="117" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B117" s="6"/>
       <c r="C117" s="4"/>
     </row>
-    <row r="118" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B118" s="6"/>
       <c r="C118" s="4"/>
     </row>
-    <row r="119" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B119" s="6"/>
       <c r="C119" s="4"/>
     </row>
-    <row r="120" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="121" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="121" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B121" s="3"/>
       <c r="C121" s="3"/>
     </row>
-    <row r="122" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B122" s="8"/>
       <c r="C122" s="9"/>
     </row>
-    <row r="123" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B123" s="8"/>
       <c r="C123" s="9"/>
     </row>
-    <row r="124" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="s">
         <v>29</v>
       </c>
@@ -1480,9 +1511,9 @@
       <selection sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="10.875" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1639,7 +1670,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1648,7 +1679,7 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1657,7 +1688,7 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1666,7 +1697,7 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1675,7 +1706,7 @@
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1684,7 +1715,7 @@
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1693,7 +1724,7 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>

</xml_diff>

<commit_message>
Finished structure of assessment files
</commit_message>
<xml_diff>
--- a/files/assesments/firstround/assesments-jacob.xlsx
+++ b/files/assesments/firstround/assesments-jacob.xlsx
@@ -9,15 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="22240" windowHeight="13440" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20500" windowHeight="7540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Peer  and self assessment" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$A$5</definedName>
   </definedNames>
@@ -34,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>Self assesment</t>
   </si>
@@ -84,22 +81,28 @@
     <t>Robert</t>
   </si>
   <si>
-    <t>Alexander</t>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magnus </t>
+  </si>
+  <si>
+    <t>Anna</t>
   </si>
   <si>
     <t>Morcel</t>
   </si>
   <si>
-    <t>Anna</t>
-  </si>
-  <si>
-    <t>Peter</t>
-  </si>
-  <si>
-    <t>Daniel</t>
+    <t xml:space="preserve">Daniel </t>
   </si>
   <si>
     <t>Magnus</t>
+  </si>
+  <si>
+    <t>Alex</t>
   </si>
 </sst>
 </file>
@@ -276,21 +279,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Peer  and self assessment"/>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -566,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C124"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -580,7 +568,7 @@
     <col min="7" max="7" width="54" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>8</v>
       </c>
@@ -598,58 +586,58 @@
       <c r="B2" s="6"/>
       <c r="C2" s="7"/>
     </row>
-    <row r="3" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="7"/>
     </row>
-    <row r="5" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="4"/>
     </row>
     <row r="9" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="4"/>
     </row>
     <row r="10" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="4"/>
@@ -682,56 +670,56 @@
     </row>
     <row r="16" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="4"/>
     </row>
     <row r="17" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="4"/>
     </row>
     <row r="18" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="4"/>
     </row>
     <row r="19" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="4"/>
     </row>
     <row r="20" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="4"/>
     </row>
     <row r="21" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="4"/>
     </row>
     <row r="22" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="4"/>
     </row>
     <row r="23" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B23" s="6"/>
       <c r="C23" s="4"/>
@@ -772,101 +760,6 @@
       <c r="B29" s="8"/>
       <c r="C29" s="9"/>
     </row>
-    <row r="30" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="50" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="65" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="66" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="67" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="68" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="70" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="72" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="73" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="74" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="76" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="77" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="78" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="79" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="81" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="82" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="83" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="84" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="85" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="86" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="87" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="88" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="89" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="90" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="91" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="92" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="93" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="94" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="95" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="96" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="97" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="98" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="99" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="100" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="101" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="102" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="103" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="104" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="105" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="106" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="107" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="108" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="109" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="110" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="111" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="112" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="113" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="114" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="115" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="116" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="117" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="118" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="119" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="120" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="121" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="122" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="123" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="124" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B27:C27"/>
@@ -883,7 +776,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please choose a grade">
           <x14:formula1>
-            <xm:f>[1]Sheet1!#REF!</xm:f>
+            <xm:f>Sheet1!$A$2:$A$5</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B11 B15:B24</xm:sqref>
         </x14:dataValidation>

</xml_diff>

<commit_message>
Added the last assesments
</commit_message>
<xml_diff>
--- a/files/assesments/firstround/assesments-jacob.xlsx
+++ b/files/assesments/firstround/assesments-jacob.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobvejlinjensen/Honeyjar/files/assesments/firstround/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lanes\OneDrive\Dokumenter\uni\2. semester\epic\files\assesments\firstround\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="20500" windowHeight="7540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="20505" windowHeight="7545" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Peer  and self assessment" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t>Self assesment</t>
   </si>
@@ -103,12 +103,18 @@
   </si>
   <si>
     <t>Alex</t>
+  </si>
+  <si>
+    <t>Very active in our online meetings, Uploaded relevant articles to github</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quick response in Discord, well formulated and active in meetings </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -556,15 +562,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.1640625" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" customWidth="1"/>
-    <col min="3" max="3" width="64.6640625" customWidth="1"/>
+    <col min="1" max="1" width="40.125" customWidth="1"/>
+    <col min="2" max="2" width="21.625" customWidth="1"/>
+    <col min="3" max="3" width="64.625" customWidth="1"/>
     <col min="7" max="7" width="54" customWidth="1"/>
   </cols>
   <sheetData>
@@ -579,7 +585,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -604,8 +610,12 @@
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="4"/>
+      <c r="B5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -614,43 +624,43 @@
       <c r="B6" s="6"/>
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="4"/>
     </row>
-    <row r="13" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>9</v>
       </c>
@@ -661,99 +671,103 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="4"/>
-    </row>
-    <row r="17" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="4"/>
     </row>
-    <row r="18" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="4"/>
     </row>
-    <row r="22" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B23" s="6"/>
       <c r="C23" s="4"/>
     </row>
-    <row r="24" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="4"/>
     </row>
-    <row r="25" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
     </row>
-    <row r="27" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="9"/>
     </row>
-    <row r="28" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="9"/>
     </row>
-    <row r="29" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>13</v>
       </c>
@@ -794,12 +808,12 @@
       <selection sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.83203125" customWidth="1"/>
+    <col min="3" max="3" width="10.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -810,7 +824,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -821,7 +835,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -832,7 +846,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -843,7 +857,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -854,7 +868,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -863,7 +877,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -872,7 +886,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -881,7 +895,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -890,7 +904,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -899,7 +913,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -908,7 +922,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -917,7 +931,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -926,7 +940,7 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -935,7 +949,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -944,7 +958,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -953,7 +967,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -962,7 +976,7 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -971,7 +985,7 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -980,7 +994,7 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -989,7 +1003,7 @@
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -998,7 +1012,7 @@
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1007,7 +1021,7 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>

</xml_diff>

<commit_message>
Updated assessment for myself
</commit_message>
<xml_diff>
--- a/files/assesments/firstround/assesments-jacob.xlsx
+++ b/files/assesments/firstround/assesments-jacob.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="20500" windowHeight="7540" tabRatio="500"/>
+    <workbookView xWindow="12980" yWindow="460" windowWidth="15820" windowHeight="12300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Peer  and self assessment" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
   <si>
     <t>Self assesment</t>
   </si>
@@ -103,6 +103,23 @@
   </si>
   <si>
     <t>Alex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I have been active in the weekly online Discord meetings - both in 
+terms of planning (Adding discussion points to the meeting agenda, taking responsibility for leading a group discussion or a walkthrough of conducted work, etc) 
+I have been reading through literature and materials uploaded
+to GiT by other project group members, and actively been adding comments and suggestions. I have been uploading relevant materials to
+GiT as well.  
+I have been responding fairly quickly to messages, both private and group announcements, on the discord platform. </t>
+  </si>
+  <si>
+    <t>Active collaborator, motivated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research, hardware setup </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Active collaboration with Ahmet about Machine learning (Including sharing  research and literature), Active collaboration with Alex and Morcel about the PoA (Including giving inputs and suggestions for conducted work), Active communication and use of GiT and Discord, </t>
   </si>
 </sst>
 </file>
@@ -556,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -583,15 +600,23 @@
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7"/>
+      <c r="B2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="3" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="4"/>
+      <c r="B3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="4" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -665,8 +690,12 @@
       <c r="A15" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="4"/>
+      <c r="B15" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="16" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
@@ -714,8 +743,12 @@
       <c r="A22" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="4"/>
+      <c r="B22" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="23" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">

</xml_diff>

<commit_message>
Merged jacobs files in - Guys remember til pull
</commit_message>
<xml_diff>
--- a/files/assesments/firstround/assesments-jacob.xlsx
+++ b/files/assesments/firstround/assesments-jacob.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
   <si>
     <t>Self assesment</t>
   </si>
@@ -112,6 +112,20 @@
   </si>
   <si>
     <t xml:space="preserve">Good use of communication programs, and making sure everybody is on the right track. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I have been active in the weekly online Discord meetings - both in 
+terms of planning (Adding discussion points to the meeting agenda, taking responsibility for leading a group discussion or a walkthrough of conducted work, etc) 
+I have been reading through literature and materials uploaded
+to GiT by other project group members, and actively been adding comments and suggestions. I have been uploading relevant materials to
+GiT as well.  
+I have been responding fairly quickly to messages, both private and group announcements, on the discord platform. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research, hardware setup </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Active collaboration with Ahmet about Machine learning (Including sharing  research and literature), Active collaboration with Alex and Morcel about the PoA (Including giving inputs and suggestions for conducted work), Active communication and use of GiT and Discord, </t>
   </si>
 </sst>
 </file>
@@ -565,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -592,15 +606,23 @@
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7"/>
+      <c r="B2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="3" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="4"/>
+      <c r="B3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="4" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -678,8 +700,12 @@
       <c r="A15" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="4"/>
+      <c r="B15" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="16" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">

</xml_diff>